<commit_message>
all Op Plan sites are done
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 08_31_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 08_31_2019.xlsx
@@ -2168,7 +2168,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2517,7 +2517,7 @@
   <dimension ref="A1:W593"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B442" sqref="B442"/>
     </sheetView>
   </sheetViews>

</xml_diff>